<commit_message>
After changing RE-START and RESUME and a few other things
</commit_message>
<xml_diff>
--- a/source/CARROT_SI.xlsx
+++ b/source/CARROT_SI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="8040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="8040" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Read me" sheetId="29" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="369">
   <si>
     <t>Advantages</t>
   </si>
@@ -87,12 +87,6 @@
 o Allows the effect of all or part of rhizodeposits on the behavior of pure microbial strains to be studied</t>
   </si>
   <si>
-    <t>Setting sterility or monoxenic conditions during plant growth</t>
-  </si>
-  <si>
-    <t>Setting sterility or monoxenic conditions when collecting rhizodeposits</t>
-  </si>
-  <si>
     <t>Warnings</t>
   </si>
   <si>
@@ -284,27 +278,6 @@
 o Integrates across diurnal variation, avoiding time-of-day bias</t>
   </si>
   <si>
-    <t>o Separates the fractions of interest, e.g. isolates soluble compounds
-o Eliminates root debris and RET
-o Reduces the number of cells in the supernatant (e.g. microbial cells if any).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">o Separates the fractions of interest, e.g. isolates soluble compounds
-o Eliminates root debris, root cells and RET
-o The filtered sample is free of microorganisms (prevention of microbial degradation)
-</t>
-  </si>
-  <si>
-    <t>o Can lead to cell lysis and the release of cellular content in the exudates
-o A part of root exudates remains trapped at the bottom of the tube
-o Does not ensure sample sterility (microorganisms may still be present in the supernatant)</t>
-  </si>
-  <si>
-    <t>o Possible retention of specific molecules on the filter, leading to a change in the composition of the exudates collected
-o A part of root exudates is lost in the retention volume of the filter
-o Contaminants may be released by the filter (e.g. from cellulose), which alters the composition of exudates and considerably hampers their chemical analysis</t>
-  </si>
-  <si>
     <t>o No risk of sample loss or contamination possibly caused by centrifugation or filtration</t>
   </si>
   <si>
@@ -604,9 +577,6 @@
 o May lack realism compared to field climatic conditions (e.g., differences in light quality and intensity)
 o Plants are often grown in pots, hydroponic, or aeroponic systems, which can alter root temperature and growth dynamics compared to field conditions (this must be carefully managed)
 o Natural climate variability (diurnal, seasonal, interannual) is usually not considered</t>
-  </si>
-  <si>
-    <t>Liquid (hydroponics) or air (aeroponics</t>
   </si>
   <si>
     <t>Agar or other gel-like substrate</t>
@@ -726,12 +696,6 @@
     <t>o Does not allow to distinguish different types of compounds
 o Most analyzers usually require at least 10-20 ml of sample
 o Concentrations below ~ 0.1 mgC L-1 are difficult to detect and quantify</t>
-  </si>
-  <si>
-    <t>o Suitable for quantifying border-like cells, with microscopy and/or flux cytometry</t>
-  </si>
-  <si>
-    <t>o Useful to localize hot spots along roots when coupled to fluorescing agents or bacteria (reporter genes) or color agents reacting with specific compounds</t>
   </si>
   <si>
     <t>1, 2</t>
@@ -881,13 +845,6 @@
 o Well-suited for initial screening of exudates</t>
   </si>
   <si>
-    <t>o Hard to set up
-o Low volume / amounts collected
-o Non-polar or hydrophobic compounds are difficult to collect
-o Does not provide a picture for the whole root system
-o If roots and solution samplers are not separated from the actual soil, quantitative analyses will be impossible (e.g. sorption); the distinction between root exudates and soil-borne compounds may require isotopic analyses</t>
-  </si>
-  <si>
     <t>o Enables to collect root exudates on specific root zones and investigate spatial and temporal variations</t>
   </si>
   <si>
@@ -935,12 +892,6 @@
 </t>
   </si>
   <si>
-    <t>o Hard to set up &amp; invasive for the investigated root
-o Only a low volume / amount can be collected in each zone
-o Does not provide a picture of the whole root system
-o If roots are not separated from the actual soil, quantitative analyses may be impossible; the distinction between root exudates and soil-borne compounds may require isotopic analyses</t>
-  </si>
-  <si>
     <r>
       <t>Direct collection of the solid growth substrate</t>
     </r>
@@ -1055,10 +1006,6 @@
   <si>
     <t>o May be required if several analyses need to be done (e.g. additional total C measurement used as a reference or for normalization issue)
 o Subsampling requires a high homogeneity in the bulk sample, which is hard to achieve with solid samples</t>
-  </si>
-  <si>
-    <t>o No separation of distinct rhizodeposits fraction
-o Particles and debris present in the sample may clog analyzers later on</t>
   </si>
   <si>
     <r>
@@ -1563,11 +1510,6 @@
     <t>o Unrealistic spatial gradient of concentration along roots
 o Non-polar or hydrophobic compounds are difficult to collect
 o The presence of nutrients/salts may cause problem for downstream analyses</t>
-  </si>
-  <si>
-    <t>o Unrealistic spatial gradient of concentration along roots
-o Non-polar or hydrophobic compounds are difficult to collect
-o If the growth substrate is actual soil, quantitative analyses are impossible, and distinguishing rhizodeposits from soil-borne compounds is virtually impossible without isotopic analyses</t>
   </si>
   <si>
     <r>
@@ -1882,21 +1824,6 @@
 o Usually requires purification and/or concentration steps</t>
   </si>
   <si>
-    <t>o Cheap
-o Allows to treat large volume</t>
-  </si>
-  <si>
-    <t>o More accurate than paper filters
-o Allows removing microorganisms (&lt; 0.2 µm)</t>
-  </si>
-  <si>
-    <t>o Less precise than syringe filters</t>
-  </si>
-  <si>
-    <t>o Low throughput
-o Limited to small samples</t>
-  </si>
-  <si>
     <t>o Typically soil or solid growth substrate (e.g. sand, glass beads)</t>
   </si>
   <si>
@@ -1906,39 +1833,7 @@
     <t>o Typically air to analyze VOC</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">o Other techniques, such as autoradiography coupled with </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>14</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C isotope labelling to localize hotspots of rhizodeposition, or image analysis of fluoescencing bacteria responding to specific substrates</t>
-    </r>
-  </si>
-  <si>
     <t>o Allows the gentle separation of cap cells and bacterial cells, and their possible recovery</t>
-  </si>
-  <si>
-    <t>o Slower than ultracentrifugation
-o Limited to small-volume samples</t>
   </si>
   <si>
     <t>o Quick
@@ -1947,16 +1842,6 @@
   <si>
     <t>o May damage cells and other structures
 o May cause sample heating</t>
-  </si>
-  <si>
-    <t>o Time-independent
-o Allows to separate and recover specific vesicles, proteins fractions or DNA/RNA fractions</t>
-  </si>
-  <si>
-    <t>o Limited to the recovery of a very specific type of rhizodeposits</t>
-  </si>
-  <si>
-    <t>v1.5 (2026-02-10)</t>
   </si>
   <si>
     <t>Plant type</t>
@@ -2617,12 +2502,137 @@
       <t xml:space="preserve"> in the companion article]</t>
     </r>
   </si>
+  <si>
+    <t>o Can lead to cell lysis and the release of cellular content in the exudates
+o A part of root exudates remains trapped at the bottom of the tube</t>
+  </si>
+  <si>
+    <t>o Separates the fractions of interest, e.g. isolates soluble compounds
+o Eliminates root debris and RET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o Separates the fractions of interest, e.g. isolates soluble compounds
+o Eliminates root debris, root cells and RET
+</t>
+  </si>
+  <si>
+    <t>o No separation of distinct rhizodeposits fraction
+o Particles and debris present in the sample may clogg analyzers later on</t>
+  </si>
+  <si>
+    <t>o Possible retention of specific molecules on the filter, leading to a change in the composition of the exudates collected
+o A part of root exudates is lost in the retention volume of the filter
+o Contaminants may be released by the filter (e.g. from cellulose), which may hamper further chemical analysis</t>
+  </si>
+  <si>
+    <t>o The pellet is often invisible with low-adhesion pellet, making it difficult to ensure a proper separation from the supernatant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o Time consuming
+o Limited to the recovery of a very specific type of rhizodeposits
+o Losses may occur during sample recovery
+</t>
+  </si>
+  <si>
+    <t>o Allows to separate and recover specific vesicles, proteins fractions or DNA/RNA fractions</t>
+  </si>
+  <si>
+    <t>o Less precise than syringe filters
+o May cause non-specific losses on the filter</t>
+  </si>
+  <si>
+    <t>o Remove particles and debris from rhizodeposits sampled from bulk soil</t>
+  </si>
+  <si>
+    <t>o Remove small particles from samples
+o Allows removing microorganisms (&lt; 0.2 µm)</t>
+  </si>
+  <si>
+    <t>o Low throughput
+o Molecules may adsorb to the filter, while contaminants may be released by it</t>
+  </si>
+  <si>
+    <t>Details &amp; warnings</t>
+  </si>
+  <si>
+    <t>o Use of microscopy (TEM, CyoSEM) or flow cytometry to count cells and or/ extracellular vesicles</t>
+  </si>
+  <si>
+    <t>o Use of light or fluorescence microscopy to observe mucilage, root cap-derived cells, RET
+o Use of MALDI to map rhizosphere compounds
+o Use of engineered bacteria to localize specific compounds
+o Use of microfluidic chips with liquid micro-junction surface sampling probe for high spatiotemporal distribution
+o Visualizing extra vesicles near the roots and/or in the rhizosphere remains challenging</t>
+  </si>
+  <si>
+    <t>o Use of 14C labelling coupled to autoradiography or 11C coupled to PET-scanner to track recently assimilated C in the rhizosphere
+o Use of 13C labelling, thin section preparation and (nano-)SIMS to track root-derived C
+o Use of dyes for localizing extracellular DNA or characterizing its structure
+o Use of dyes or planar optodes to map pH or redox variations within the rhizosphere</t>
+  </si>
+  <si>
+    <t>Liquid (hydroponics) or air (aeroponics)</t>
+  </si>
+  <si>
+    <t>o Hard to set up &amp; invasive for the investigated root
+o Only a low volume / amount can be collected in each zone
+o Does not provide a picture of the whole root system
+o If roots are not separated from the actual soil, quantitative analyses may be impossible; the distinction between root exudates and soil-borne compounds may require isotopic analyses and careful timing</t>
+  </si>
+  <si>
+    <t>o Hard to set up
+o Low volume / amounts collected
+o Non-polar or hydrophobic compounds are difficult to collect
+o Does not provide a picture for the whole root system
+o If roots and solution samplers are not separated from the actual soil, quantitative analyses will be impossible (e.g. sorption); the distinction between root exudates and soil-borne compounds may require isotopic analyses and caeful timing</t>
+  </si>
+  <si>
+    <t>o Unrealistic spatial gradient of concentration along roots
+o Non-polar or hydrophobic compounds are difficult to collect
+o If the growth substrate is actual soil, quantitative analyses are impossible, and distinguishing rhizodeposits from soil-borne compounds is virtually impossible without isotopic analyses and careful timing</t>
+  </si>
+  <si>
+    <t>o Required for stopping microbial activity, and for maximal conservation (e.g. DNA)
+o WATCH OUT: if a liquid sample has been frozen, some precipitation may have occured and cause analytical bias or cloging issues!</t>
+  </si>
+  <si>
+    <t>v1.5 (2026-02-23)</t>
+  </si>
+  <si>
+    <t>Non-sterile environment during plant growth</t>
+  </si>
+  <si>
+    <t>o Natural plant-microbe interactions and their effects on plant growth are taken into accounts
+o Allows a realistic assessment of rhizodeposition dynamics during plant growth (e.g. with isotope labelling)
+o Avoids artefacts introduced by soil sterilization</t>
+  </si>
+  <si>
+    <t>o Incompatible with the collection of rhizodeposits in fully sterile conditions
+o Less controllable and reproducible than in sterile environment</t>
+  </si>
+  <si>
+    <t>Non-sterile conditions during rhizodeposit collection</t>
+  </si>
+  <si>
+    <t>Sterile conditions when collecting rhizodeposits</t>
+  </si>
+  <si>
+    <t>Sterile, monoxenic or gnotobiotic conditions during plant growth</t>
+  </si>
+  <si>
+    <t>o High risk of rhizodeposits degradation or alteration by microorganisms
+o Risk of rhizodeposits contamination by microbial products
+o Using a short collection period is crucial to minimize the impact of microbial activity, which lowers the amount of rhizodeposits that can be collected</t>
+  </si>
+  <si>
+    <t>o Natural plant-microbe interactions and their effects on rhizodeposition are taken into accounts</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2746,15 +2756,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <vertAlign val="superscript"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2980,6 +2981,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2988,9 +2992,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3275,7 +3276,9 @@
   <sheetPr codeName="Feuil28"/>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3286,10 +3289,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="45" t="s">
-        <v>316</v>
+        <v>78</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>360</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
@@ -3305,40 +3308,40 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>340</v>
-      </c>
-      <c r="C3" s="42"/>
+        <v>79</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>318</v>
+      </c>
+      <c r="C3" s="43"/>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="25"/>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="25"/>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
@@ -3352,56 +3355,56 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="26" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="26" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="42"/>
+      <c r="A13" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="43"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="43"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3417,10 +3420,10 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil7"/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3433,52 +3436,67 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>322</v>
+        <v>300</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A2" s="30">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="30">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="B3" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>347</v>
+      <c r="C4" s="10" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil29"/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3491,38 +3509,52 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>322</v>
+        <v>300</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A2" s="30">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="30">
         <v>2</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="19" t="s">
+      <c r="B3" s="18" t="s">
+        <v>365</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="19" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="D3" s="19" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>347</v>
+      <c r="C4" s="10" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -3552,13 +3584,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -3569,13 +3601,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="165.6" x14ac:dyDescent="0.3">
@@ -3583,13 +3615,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -3597,13 +3629,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3611,7 +3643,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>348</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -3637,13 +3669,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -3654,13 +3686,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -3668,13 +3700,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
@@ -3682,13 +3714,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3696,13 +3728,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3710,7 +3742,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>349</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -3737,13 +3769,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -3754,27 +3786,27 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3782,7 +3814,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>349</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -3808,13 +3840,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -3825,13 +3857,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
@@ -3839,18 +3871,18 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C4" s="10" t="s">
-        <v>350</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -3876,13 +3908,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>324</v>
+        <v>302</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3890,10 +3922,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3901,10 +3933,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3912,10 +3944,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3923,7 +3955,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>341</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -3938,7 +3970,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3949,13 +3981,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -3963,16 +3995,16 @@
     </row>
     <row r="2" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
@@ -3980,27 +4012,27 @@
         <v>3</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="144" x14ac:dyDescent="0.3">
       <c r="A4" s="30">
         <v>4</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>177</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
@@ -4008,13 +4040,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
@@ -4022,13 +4054,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>259</v>
+        <v>358</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
@@ -4036,13 +4068,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -4050,13 +4082,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -4064,13 +4096,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="102.6" x14ac:dyDescent="0.3">
@@ -4078,19 +4110,19 @@
         <v>10</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="C11" s="10" t="s">
-        <v>341</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -4116,13 +4148,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -4133,13 +4165,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
@@ -4147,13 +4179,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -4161,19 +4193,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>351</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -4199,13 +4231,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>325</v>
+        <v>303</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -4216,13 +4248,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
@@ -4230,13 +4262,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
@@ -4244,13 +4276,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
@@ -4258,19 +4290,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>352</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -4293,31 +4325,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="44"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="44"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="44"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4345,13 +4377,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>326</v>
+        <v>304</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -4359,10 +4391,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -4370,10 +4402,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -4381,16 +4413,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>341</v>
+        <v>319</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -4417,13 +4449,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>327</v>
+        <v>305</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
@@ -4431,10 +4463,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -4442,16 +4474,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>341</v>
+        <v>319</v>
       </c>
       <c r="D4" s="4"/>
     </row>
@@ -4466,7 +4498,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4478,13 +4510,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -4492,10 +4524,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>246</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -4503,10 +4535,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4514,10 +4546,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
@@ -4525,16 +4557,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>353</v>
+        <v>331</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -4549,7 +4581,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4560,44 +4592,44 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>328</v>
+        <v>306</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A2" s="30">
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>70</v>
+        <v>340</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A3" s="30">
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>71</v>
+        <v>341</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>73</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -4605,19 +4637,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>200</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>354</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -4631,7 +4663,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4643,30 +4675,30 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>329</v>
+        <v>307</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="30">
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>311</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -4674,33 +4706,33 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="69" x14ac:dyDescent="0.3">
       <c r="A4" s="30">
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>314</v>
+        <v>346</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>315</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>354</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -4714,9 +4746,7 @@
   <sheetPr codeName="Feuil20"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4727,13 +4757,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>330</v>
+        <v>308</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -4744,33 +4774,33 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>302</v>
+        <v>348</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="30">
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>303</v>
+        <v>349</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>305</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>354</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -4797,13 +4827,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>331</v>
+        <v>309</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -4814,13 +4844,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
@@ -4828,13 +4858,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
@@ -4842,19 +4872,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>355</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -4880,13 +4910,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>332</v>
+        <v>310</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -4897,13 +4927,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -4911,19 +4941,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>355</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -4949,13 +4979,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>333</v>
+        <v>311</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -4966,13 +4996,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -4980,13 +5010,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -4994,19 +5024,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>355</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -5032,13 +5062,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>334</v>
+        <v>312</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -5049,13 +5079,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -5063,13 +5093,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5077,19 +5107,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>355</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -5115,13 +5145,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
@@ -5129,10 +5159,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -5140,10 +5170,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -5151,10 +5181,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
@@ -5162,10 +5192,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -5173,10 +5203,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -5184,10 +5214,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -5198,7 +5228,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>341</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -5224,13 +5254,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5238,10 +5268,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5249,10 +5279,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -5260,10 +5290,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
@@ -5271,16 +5301,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>356</v>
+        <v>334</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -5307,13 +5337,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5321,10 +5351,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5332,10 +5362,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5343,10 +5373,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
@@ -5354,16 +5384,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>345</v>
+        <v>323</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -5391,10 +5421,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>335</v>
+        <v>313</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>0</v>
@@ -5408,13 +5438,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
@@ -5422,13 +5452,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="165.6" x14ac:dyDescent="0.3">
@@ -5436,13 +5466,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -5450,19 +5480,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>357</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -5488,13 +5518,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -5505,13 +5535,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="220.8" x14ac:dyDescent="0.3">
@@ -5519,19 +5549,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>358</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -5559,13 +5589,13 @@
   <sheetData>
     <row r="1" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>337</v>
+        <v>315</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -5576,13 +5606,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="E2" s="4"/>
     </row>
@@ -5591,13 +5621,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
@@ -5605,19 +5635,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>358</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -5643,13 +5673,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>339</v>
+        <v>317</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -5660,13 +5690,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="138" x14ac:dyDescent="0.3">
@@ -5674,19 +5704,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>359</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -5699,7 +5729,9 @@
   <sheetPr codeName="Feuil27"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5709,13 +5741,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>338</v>
+        <v>316</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>195</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -5723,38 +5755,38 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A3" s="30">
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="69" x14ac:dyDescent="0.3">
       <c r="A4" s="30">
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>309</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>360</v>
+        <v>338</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -5781,13 +5813,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
@@ -5795,10 +5827,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
@@ -5806,10 +5838,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
@@ -5817,10 +5849,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -5828,10 +5860,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -5839,10 +5871,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -5850,10 +5882,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
@@ -5861,15 +5893,15 @@
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" s="10" t="s">
-        <v>341</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -5895,13 +5927,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>317</v>
+        <v>295</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
@@ -5909,10 +5941,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="110.4" x14ac:dyDescent="0.3">
@@ -5920,10 +5952,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="138" x14ac:dyDescent="0.3">
@@ -5931,10 +5963,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
@@ -5942,10 +5974,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -5956,7 +5988,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>342</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -5983,13 +6015,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>318</v>
+        <v>296</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -6000,13 +6032,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
@@ -6014,13 +6046,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
@@ -6028,13 +6060,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -6045,7 +6077,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>343</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -6071,13 +6103,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>319</v>
+        <v>297</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -6085,30 +6117,30 @@
     </row>
     <row r="2" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -6116,7 +6148,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>344</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -6134,7 +6166,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6146,13 +6178,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -6163,27 +6195,27 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="138" x14ac:dyDescent="0.3">
@@ -6191,33 +6223,33 @@
         <v>4</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>113</v>
+        <v>355</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="13"/>
       <c r="C6" s="10" t="s">
-        <v>345</v>
+        <v>323</v>
       </c>
       <c r="D6" s="14"/>
     </row>
@@ -6245,13 +6277,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>321</v>
+        <v>299</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -6262,13 +6294,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -6276,13 +6308,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
@@ -6290,13 +6322,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="72" x14ac:dyDescent="0.3">
@@ -6304,19 +6336,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="13"/>
       <c r="C6" s="10" t="s">
-        <v>346</v>
+        <v>324</v>
       </c>
       <c r="D6" s="14"/>
     </row>

</xml_diff>

<commit_message>
After modifying RESTART and RESUME, updating the souce files, the manual and the README
</commit_message>
<xml_diff>
--- a/source/CARROT_SI.xlsx
+++ b/source/CARROT_SI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="8040" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="8040" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Read me" sheetId="29" r:id="rId1"/>
@@ -758,11 +758,6 @@
 o Transparent plastic (ex : polycarbonate) allows to monitor root growth</t>
   </si>
   <si>
-    <t>o Low-quality plastics may release germination- or growth-inhibitors, and contaminate the growth material and the rhizodeposits
-o Microparticles may be absorbed by roots or retained at the root surface
-o Sensitive to physical constraints (scratches…)</t>
-  </si>
-  <si>
     <t>o Relatively cheap
 o Low risk of contamination</t>
   </si>
@@ -770,11 +765,6 @@
     <t>o Heavy
 o Limited in possible volumes and designs
 o May adsorb nutrients and/or rhizodeposits</t>
-  </si>
-  <si>
-    <t>o Expensive
-o Heavy and fragile
-o Particular designs require specialized glassmakers</t>
   </si>
   <si>
     <t>o Chemically inert towards organics and macronutrients
@@ -1115,20 +1105,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>(ex: PE, PP)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Growing plants in ceramic containers </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(ex: terracotta)</t>
     </r>
   </si>
   <si>
@@ -2626,6 +2602,32 @@
   </si>
   <si>
     <t>o Natural plant-microbe interactions and their effects on rhizodeposition are taken into accounts</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Growing plants in ceramic containers </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(ex: terracotta, glazed ceramics)</t>
+    </r>
+  </si>
+  <si>
+    <t>o Low-quality plastics may release germination- or growth-inhibitors, and contaminate the growth material and the rhizodeposits
+o Microparticles may be absorbed by roots or retained at the root surface
+o Sensitive to physical constraints (scratches…)
+o If transparent: roots should always grow in the dark (use light-shielding cover)</t>
+  </si>
+  <si>
+    <t>o Expensive
+o Heavy and fragile
+o Particular designs require specialized glassmakers
+o Roots should always grown in the dark (use light-shielding cover)</t>
   </si>
 </sst>
 </file>
@@ -3292,7 +3294,7 @@
         <v>78</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
@@ -3311,7 +3313,7 @@
         <v>79</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C3" s="43"/>
       <c r="D3" s="25"/>
@@ -3439,7 +3441,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -3453,13 +3455,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
@@ -3467,7 +3469,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>5</v>
@@ -3481,7 +3483,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -3495,7 +3497,7 @@
   <sheetPr codeName="Feuil29"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -3512,7 +3514,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -3526,13 +3528,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>364</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>368</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
@@ -3540,13 +3542,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3554,7 +3556,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -3601,7 +3603,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>115</v>
@@ -3629,7 +3631,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>119</v>
@@ -3643,7 +3645,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -3656,9 +3658,7 @@
   <sheetPr codeName="Feuil10"/>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3672,7 +3672,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -3681,46 +3681,46 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A2" s="30">
         <v>1</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C2" s="39" t="s">
         <v>147</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A3" s="30">
         <v>2</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>197</v>
+        <v>366</v>
       </c>
       <c r="C3" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="D3" s="39" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A4" s="30">
         <v>3</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>151</v>
+        <v>368</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3728,13 +3728,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3742,7 +3742,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -3772,7 +3772,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -3786,13 +3786,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
@@ -3800,13 +3800,13 @@
         <v>145</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3814,7 +3814,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -3857,13 +3857,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
@@ -3871,18 +3871,18 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C4" s="10" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -3911,7 +3911,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>121</v>
@@ -3922,10 +3922,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3933,10 +3933,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3944,10 +3944,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3955,7 +3955,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -3998,13 +3998,13 @@
         <v>136</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
@@ -4012,13 +4012,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="C3" s="28" t="s">
-        <v>172</v>
-      </c>
       <c r="D3" s="28" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="144" x14ac:dyDescent="0.3">
@@ -4026,13 +4026,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
@@ -4040,13 +4040,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
@@ -4054,13 +4054,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
@@ -4071,10 +4071,10 @@
         <v>125</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -4082,13 +4082,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -4096,13 +4096,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>126</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="102.6" x14ac:dyDescent="0.3">
@@ -4110,19 +4110,19 @@
         <v>10</v>
       </c>
       <c r="B10" s="40" t="s">
+        <v>174</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>176</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="C11" s="10" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -4151,7 +4151,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -4165,13 +4165,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
@@ -4179,13 +4179,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -4193,19 +4193,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -4234,7 +4234,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -4248,7 +4248,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>64</v>
@@ -4262,10 +4262,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>66</v>
@@ -4276,13 +4276,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>67</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
@@ -4290,19 +4290,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>181</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -4380,7 +4380,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>122</v>
@@ -4394,7 +4394,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -4405,7 +4405,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -4416,13 +4416,13 @@
         <v>29</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -4452,7 +4452,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>122</v>
@@ -4466,7 +4466,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -4477,13 +4477,13 @@
         <v>31</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D4" s="4"/>
     </row>
@@ -4527,7 +4527,7 @@
         <v>33</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -4538,7 +4538,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4549,7 +4549,7 @@
         <v>35</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
@@ -4560,13 +4560,13 @@
         <v>36</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -4595,7 +4595,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -4612,10 +4612,10 @@
         <v>37</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
@@ -4626,10 +4626,10 @@
         <v>38</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -4643,13 +4643,13 @@
         <v>68</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -4678,7 +4678,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -4695,10 +4695,10 @@
         <v>40</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -4709,10 +4709,10 @@
         <v>41</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -4723,16 +4723,16 @@
         <v>127</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -4760,7 +4760,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -4777,10 +4777,10 @@
         <v>129</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -4791,16 +4791,16 @@
         <v>128</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -4830,7 +4830,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -4844,13 +4844,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>209</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
@@ -4858,13 +4858,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>213</v>
-      </c>
       <c r="D3" s="23" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
@@ -4875,16 +4875,16 @@
         <v>76</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -4913,7 +4913,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -4927,13 +4927,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C2" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>219</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -4941,19 +4941,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>218</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>220</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -4982,7 +4982,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -4999,10 +4999,10 @@
         <v>42</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5013,10 +5013,10 @@
         <v>44</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5027,16 +5027,16 @@
         <v>75</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -5065,7 +5065,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -5079,13 +5079,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C2" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>219</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -5096,10 +5096,10 @@
         <v>43</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5110,16 +5110,16 @@
         <v>77</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -5228,7 +5228,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -5271,7 +5271,7 @@
         <v>33</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5282,7 +5282,7 @@
         <v>34</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -5293,7 +5293,7 @@
         <v>35</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
@@ -5304,13 +5304,13 @@
         <v>36</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -5393,7 +5393,7 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -5424,7 +5424,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>0</v>
@@ -5480,19 +5480,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -5521,7 +5521,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -5538,10 +5538,10 @@
         <v>52</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="220.8" x14ac:dyDescent="0.3">
@@ -5552,16 +5552,16 @@
         <v>53</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -5592,7 +5592,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -5606,13 +5606,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E2" s="4"/>
     </row>
@@ -5621,13 +5621,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
@@ -5635,19 +5635,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -5676,7 +5676,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -5690,13 +5690,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>236</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="138" x14ac:dyDescent="0.3">
@@ -5704,19 +5704,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="C3" s="21" t="s">
-        <v>240</v>
-      </c>
       <c r="D3" s="21" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -5744,10 +5744,10 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -5758,7 +5758,7 @@
         <v>54</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
@@ -5769,7 +5769,7 @@
         <v>55</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -5780,13 +5780,13 @@
         <v>56</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -5819,7 +5819,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
@@ -5901,7 +5901,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" s="10" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -5930,7 +5930,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>122</v>
@@ -5988,7 +5988,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -6018,7 +6018,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -6060,7 +6060,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>101</v>
@@ -6077,7 +6077,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -6106,7 +6106,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -6120,10 +6120,10 @@
         <v>136</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>104</v>
@@ -6134,7 +6134,7 @@
         <v>137</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>105</v>
@@ -6148,7 +6148,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -6181,7 +6181,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -6195,7 +6195,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>111</v>
@@ -6209,10 +6209,10 @@
         <v>145</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>112</v>
@@ -6226,7 +6226,7 @@
         <v>107</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>110</v>
@@ -6237,7 +6237,7 @@
         <v>146</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>108</v>
@@ -6249,7 +6249,7 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="13"/>
       <c r="C6" s="10" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D6" s="14"/>
     </row>
@@ -6280,7 +6280,7 @@
         <v>138</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>124</v>
@@ -6294,13 +6294,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -6308,13 +6308,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>259</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
@@ -6322,13 +6322,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="72" x14ac:dyDescent="0.3">
@@ -6336,19 +6336,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="13"/>
       <c r="C6" s="10" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D6" s="14"/>
     </row>

</xml_diff>

<commit_message>
After minor modifications of source files and of the manual and README
</commit_message>
<xml_diff>
--- a/source/CARROT_SI.xlsx
+++ b/source/CARROT_SI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="8040" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="Read me" sheetId="29" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="368">
   <si>
     <t>Advantages</t>
   </si>
@@ -69,11 +69,6 @@
   </si>
   <si>
     <t>o High representativeness of the rhizosphere microenvironment (microbial communities, soil mechanical impedance, aeration)</t>
-  </si>
-  <si>
-    <t>o More replicable: the microbial environment is easily controlled
-o Allows studying the interactions with one single group of microorganisms (monoxenic)
-o Compatible with a collection of rhizodeposits in sterile conditions</t>
   </si>
   <si>
     <t>o Unrealistic: sterile conditions do not exist in the environment
@@ -333,119 +328,6 @@
   <si>
     <t>AUTHORSHIP
  &amp; LICENSE</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">This works originates from discussions held within the French network </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>RhizosPHARE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and the previous project</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> PHARE(2021-2022) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">funded by INRAE.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Conception &amp; programming:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Frédéric Rees
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Writing, editing &amp; testing:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Frédéric Rees, Sylvain Chéreau, Alexandre de Saint Germain, Sylvie Dinant, Virginie Lauvergeat, Barbara Pawlak, Jean-Benoît Peltier, François Perreau, Emmanuelle Personeni, Gabin Piton, Jean-Bernard Pouvreau, Aude Tixier, Anouk Zancarini, Agnès Attard
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>License:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> CeCILL-C</t>
-    </r>
   </si>
   <si>
     <t>Undocumented</t>
@@ -2572,9 +2454,6 @@
 o WATCH OUT: if a liquid sample has been frozen, some precipitation may have occured and cause analytical bias or cloging issues!</t>
   </si>
   <si>
-    <t>v1.5 (2026-02-23)</t>
-  </si>
-  <si>
     <t>Non-sterile environment during plant growth</t>
   </si>
   <si>
@@ -2628,6 +2507,124 @@
 o Heavy and fragile
 o Particular designs require specialized glassmakers
 o Roots should always grown in the dark (use light-shielding cover)</t>
+  </si>
+  <si>
+    <t>o More replicable: the microbial environment is easily controlled
+o Allows studying the interactions with one single group or a synthetic community of microorganisms (monoxenic or gnotobiotic)
+o Compatible with a collection of rhizodeposits in sterile conditions</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This works originates from discussions held within the French network </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RhizosPHARE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and the previous project</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> PHARE </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(2021-2022) funded by INRAE.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Conception &amp; programming:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Frédéric Rees
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Writing, editing &amp; testing:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Frédéric Rees, Sylvain Chéreau, Alexandre de Saint Germain, Sylvie Dinant, Virginie Lauvergeat, Barbara Pawlak, Jean-Benoît Peltier, François Perreau, Emmanuelle Personeni, Gabin Piton, Jean-Bernard Pouvreau, Aude Tixier, Anouk Zancarini, Agnès Attard
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>License:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> CeCILL-C</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2983,9 +2980,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2994,6 +2988,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3278,9 +3275,7 @@
   <sheetPr codeName="Feuil28"/>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3291,10 +3286,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>357</v>
+        <v>77</v>
+      </c>
+      <c r="B1" s="45">
+        <v>46078</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
@@ -3310,40 +3305,40 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="43" t="s">
-        <v>315</v>
-      </c>
-      <c r="C3" s="43"/>
+        <v>78</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>313</v>
+      </c>
+      <c r="C3" s="42"/>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
       <c r="D5" s="25"/>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="25"/>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
@@ -3357,56 +3352,56 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="C9" s="27" t="s">
         <v>81</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" s="26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="43"/>
+      <c r="A13" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="42" t="s">
+        <v>367</v>
+      </c>
+      <c r="C13" s="42"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="44"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
+      <c r="A14" s="43"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3424,9 +3419,7 @@
   <sheetPr codeName="Feuil7"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3438,13 +3431,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -3455,13 +3448,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
@@ -3469,13 +3462,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3483,7 +3476,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -3511,13 +3504,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -3528,13 +3521,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>362</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>361</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>365</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
@@ -3542,13 +3535,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3556,7 +3549,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -3586,13 +3579,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -3603,13 +3596,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="165.6" x14ac:dyDescent="0.3">
@@ -3617,13 +3610,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -3631,13 +3624,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3645,7 +3638,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -3658,7 +3651,7 @@
   <sheetPr codeName="Feuil10"/>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3669,13 +3662,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -3686,13 +3679,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
@@ -3700,13 +3693,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
@@ -3714,13 +3707,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3728,13 +3721,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3742,7 +3735,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -3769,13 +3762,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -3786,27 +3779,27 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3814,7 +3807,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -3840,13 +3833,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -3857,13 +3850,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
@@ -3871,18 +3864,18 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C4" s="10" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -3908,13 +3901,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3922,10 +3915,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3933,10 +3926,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3944,10 +3937,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3955,7 +3948,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -3981,13 +3974,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -3995,16 +3988,16 @@
     </row>
     <row r="2" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
@@ -4012,13 +4005,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="C3" s="28" t="s">
-        <v>170</v>
-      </c>
       <c r="D3" s="28" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="144" x14ac:dyDescent="0.3">
@@ -4026,13 +4019,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
@@ -4040,13 +4033,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
@@ -4054,13 +4047,13 @@
         <v>6</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
@@ -4068,13 +4061,13 @@
         <v>7</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -4082,13 +4075,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -4096,13 +4089,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="102.6" x14ac:dyDescent="0.3">
@@ -4110,19 +4103,19 @@
         <v>10</v>
       </c>
       <c r="B10" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>174</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="C11" s="10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -4148,13 +4141,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -4165,13 +4158,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
@@ -4179,13 +4172,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3" s="28" t="s">
         <v>249</v>
-      </c>
-      <c r="C3" s="28" t="s">
-        <v>250</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -4193,19 +4186,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -4231,13 +4224,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -4248,13 +4241,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C2" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>64</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
@@ -4262,13 +4255,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>204</v>
-      </c>
       <c r="D3" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="124.2" x14ac:dyDescent="0.3">
@@ -4276,13 +4269,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>203</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
@@ -4290,19 +4283,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>179</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -4325,31 +4318,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4377,13 +4370,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -4391,10 +4384,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -4402,10 +4395,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -4413,16 +4406,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -4449,13 +4442,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
@@ -4463,10 +4456,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
@@ -4474,16 +4467,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D4" s="4"/>
     </row>
@@ -4510,13 +4503,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -4524,10 +4517,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -4535,10 +4528,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4546,10 +4539,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
@@ -4557,16 +4550,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -4592,13 +4585,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -4609,13 +4602,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
@@ -4623,13 +4616,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>338</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -4637,19 +4630,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -4675,13 +4668,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -4692,13 +4685,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -4706,13 +4699,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -4720,19 +4713,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -4757,13 +4750,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -4774,13 +4767,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -4788,19 +4781,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -4827,13 +4820,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -4844,13 +4837,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>206</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>208</v>
-      </c>
       <c r="D2" s="23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
@@ -4858,13 +4851,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
@@ -4872,19 +4865,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -4910,13 +4903,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -4927,13 +4920,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>216</v>
-      </c>
       <c r="D2" s="23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -4941,19 +4934,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="C3" s="23" t="s">
-        <v>217</v>
-      </c>
       <c r="D3" s="23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -4979,13 +4972,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -4996,13 +4989,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5010,13 +5003,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5024,19 +5017,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -5062,13 +5055,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -5079,13 +5072,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>216</v>
-      </c>
       <c r="D2" s="23" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -5093,13 +5086,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5107,19 +5100,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -5145,13 +5138,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
@@ -5159,10 +5152,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -5170,10 +5163,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -5181,10 +5174,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
@@ -5192,10 +5185,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -5203,10 +5196,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -5214,10 +5207,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -5228,7 +5221,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -5254,13 +5247,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5268,10 +5261,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5279,10 +5272,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -5290,10 +5283,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
@@ -5301,16 +5294,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -5337,13 +5330,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5351,10 +5344,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5362,10 +5355,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
@@ -5373,10 +5366,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="55.2" x14ac:dyDescent="0.3">
@@ -5384,16 +5377,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -5421,10 +5414,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>0</v>
@@ -5438,13 +5431,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="D2" s="21" t="s">
         <v>70</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
@@ -5452,13 +5445,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="165.6" x14ac:dyDescent="0.3">
@@ -5466,13 +5459,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="21" t="s">
         <v>73</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -5480,19 +5473,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
+        <v>276</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>278</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -5518,13 +5511,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -5535,13 +5528,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="220.8" x14ac:dyDescent="0.3">
@@ -5549,19 +5542,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -5589,13 +5582,13 @@
   <sheetData>
     <row r="1" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -5606,13 +5599,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E2" s="4"/>
     </row>
@@ -5621,13 +5614,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
@@ -5635,19 +5628,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -5673,13 +5666,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -5690,13 +5683,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="C2" s="21" t="s">
-        <v>235</v>
-      </c>
       <c r="D2" s="21" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="138" x14ac:dyDescent="0.3">
@@ -5704,19 +5697,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -5741,13 +5734,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -5755,10 +5748,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
@@ -5766,10 +5759,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="69" x14ac:dyDescent="0.3">
@@ -5777,16 +5770,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D5" s="4"/>
     </row>
@@ -5813,13 +5806,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
@@ -5827,10 +5820,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
@@ -5838,10 +5831,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
@@ -5849,10 +5842,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -5860,10 +5853,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -5871,10 +5864,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
@@ -5882,10 +5875,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
@@ -5893,15 +5886,15 @@
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" s="10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -5927,13 +5920,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
@@ -5941,10 +5934,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="110.4" x14ac:dyDescent="0.3">
@@ -5952,10 +5945,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="138" x14ac:dyDescent="0.3">
@@ -5963,10 +5956,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
@@ -5974,10 +5967,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -5988,7 +5981,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -6015,13 +6008,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -6032,13 +6025,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
@@ -6046,13 +6039,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="110.4" x14ac:dyDescent="0.3">
@@ -6060,13 +6053,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -6077,7 +6070,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -6103,13 +6096,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -6117,30 +6110,30 @@
     </row>
     <row r="2" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>191</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -6148,7 +6141,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -6178,13 +6171,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -6195,27 +6188,27 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="138" x14ac:dyDescent="0.3">
@@ -6223,33 +6216,33 @@
         <v>4</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="151.80000000000001" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="13"/>
       <c r="C6" s="10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D6" s="14"/>
     </row>
@@ -6277,13 +6270,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -6294,13 +6287,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -6308,13 +6301,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="96.6" x14ac:dyDescent="0.3">
@@ -6322,13 +6315,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="41" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>264</v>
-      </c>
       <c r="D4" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="72" x14ac:dyDescent="0.3">
@@ -6336,19 +6329,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B6" s="13"/>
       <c r="C6" s="10" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D6" s="14"/>
     </row>

</xml_diff>